<commit_message>
basic import function is now implemented
</commit_message>
<xml_diff>
--- a/Hosts-Example.xlsx
+++ b/Hosts-Example.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="40">
   <si>
     <t>address</t>
   </si>
@@ -130,6 +130,15 @@
   </si>
   <si>
     <t>testing</t>
+  </si>
+  <si>
+    <t>max_check_attempts</t>
+  </si>
+  <si>
+    <t>notifications_enabled</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -540,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -558,9 +567,11 @@
     <col min="8" max="8" width="25.33203125" customWidth="1"/>
     <col min="9" max="9" width="26.1640625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -591,8 +602,14 @@
       <c r="J1" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="16" thickTop="1">
+      <c r="K1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="16" thickTop="1">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -623,8 +640,11 @@
       <c r="J2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -655,8 +675,14 @@
       <c r="J3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3">
+        <v>55</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -687,8 +713,14 @@
       <c r="J4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -719,8 +751,14 @@
       <c r="J5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -751,8 +789,11 @@
       <c r="J6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -783,8 +824,11 @@
       <c r="J7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -815,8 +859,14 @@
       <c r="J8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -847,8 +897,14 @@
       <c r="J9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -879,8 +935,14 @@
       <c r="J10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -910,6 +972,12 @@
       </c>
       <c r="J11" t="s">
         <v>36</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
service-cloning does now work
</commit_message>
<xml_diff>
--- a/Hosts-Example.xlsx
+++ b/Hosts-Example.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="42">
   <si>
     <t>address</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>true</t>
+  </si>
+  <si>
+    <t>CLONEFROM</t>
+  </si>
+  <si>
+    <t>Linuxtest01</t>
   </si>
 </sst>
 </file>
@@ -549,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -571,7 +577,7 @@
     <col min="12" max="12" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -608,8 +614,11 @@
       <c r="L1" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="16" thickTop="1">
+    <row r="2" spans="1:13" ht="16" thickTop="1">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -644,7 +653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -682,7 +691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -719,8 +728,11 @@
       <c r="L4">
         <v>1</v>
       </c>
+      <c r="M4" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -751,14 +763,11 @@
       <c r="J5" t="s">
         <v>36</v>
       </c>
-      <c r="K5">
-        <v>5</v>
-      </c>
       <c r="L5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -793,7 +802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -828,7 +837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -866,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -904,7 +913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -942,7 +951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>18</v>
       </c>

</xml_diff>